<commit_message>
Small fixes to folder path
</commit_message>
<xml_diff>
--- a/Config.template.xlsx
+++ b/Config.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMK\Harjoittelu\UiPath\TravelExpenseAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94439E49-D79D-40AB-AB5C-B93C5CCDC695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB8A0D0-B9A2-43EA-9EEA-227769F2A8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Key</t>
   </si>
@@ -101,17 +101,26 @@
     <t>Root path for the project</t>
   </si>
   <si>
-    <t>&lt;set via environment variable&gt;</t>
-  </si>
-  <si>
-    <t>your.email@example.com</t>
+    <t>EmailBodyTemplate</t>
+  </si>
+  <si>
+    <t>Please find attached travel expense report from today's inputs.</t>
+  </si>
+  <si>
+    <t>Email message</t>
+  </si>
+  <si>
+    <t>&lt;add root for the project's basefolder&gt;</t>
+  </si>
+  <si>
+    <t>&lt;add email address to which the report is sent&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,9 +141,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -161,13 +175,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -284,17 +298,13 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="5" tint="0.79998168889431442"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -470,8 +480,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{081F6D4F-E21F-451F-848E-811F42BB6F7C}" name="Table2" displayName="Table2" ref="A1:C2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:C2" xr:uid="{081F6D4F-E21F-451F-848E-811F42BB6F7C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{081F6D4F-E21F-451F-848E-811F42BB6F7C}" name="Table2" displayName="Table2" ref="A1:C3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C3" xr:uid="{081F6D4F-E21F-451F-848E-811F42BB6F7C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D9F2F91D-5A79-41E0-B33A-7864C8886283}" name="Key" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{9003EAF3-6E1A-4A92-8EC0-08FE200E15B9}" name="Value" dataDxfId="6"/>
@@ -758,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7E18BF-5F06-48B8-BF70-0AD54A44CDF0}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -785,8 +795,8 @@
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
@@ -846,10 +856,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F47627-0DAA-4E5B-BB18-3A76E2EC37BF}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -876,10 +886,21 @@
         <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>